<commit_message>
Added harangad missed photo
</commit_message>
<xml_diff>
--- a/src/player_data.xlsx
+++ b/src/player_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yashj\Programming\gradtag\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D356B8A1-B999-4514-97A5-A2474F6B3C78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33581DB6-8AE6-49AB-863D-9E553AADA795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="638">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="638">
   <si>
     <t>Id</t>
   </si>
@@ -1003,9 +1003,6 @@
     <t>Harnagad Sidhu</t>
   </si>
   <si>
-    <t>angad_ssidhu</t>
-  </si>
-  <si>
     <t>adam.bennett@surreyschools.ca</t>
   </si>
   <si>
@@ -1934,6 +1931,9 @@
   </si>
   <si>
     <t>unkown</t>
+  </si>
+  <si>
+    <t>https://sd36-my.sharepoint.com/personal/yash_jain_surreyschools_ca/Documents/Apps/Microsoft%20Forms/Grad%20Tag/Question/Harangad_IMG_GT.jpeg</t>
   </si>
 </sst>
 </file>
@@ -2024,7 +2024,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2054,6 +2054,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2378,8 +2379,8 @@
   </sheetPr>
   <dimension ref="A1:G170"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F171" sqref="F171"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="F86" sqref="F86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4326,10 +4327,12 @@
       <c r="E86" s="16" t="s">
         <v>326</v>
       </c>
-      <c r="F86" s="7" t="s">
-        <v>327</v>
-      </c>
-      <c r="G86" s="7"/>
+      <c r="F86" s="11" t="s">
+        <v>637</v>
+      </c>
+      <c r="G86" s="17" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="87" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" s="12">
@@ -4342,16 +4345,16 @@
         <v>45698.525694444441</v>
       </c>
       <c r="D87" s="14" t="s">
+        <v>327</v>
+      </c>
+      <c r="E87" s="10" t="s">
         <v>328</v>
       </c>
-      <c r="E87" s="10" t="s">
+      <c r="F87" s="12" t="s">
         <v>329</v>
       </c>
-      <c r="F87" s="12" t="s">
+      <c r="G87" s="12" t="s">
         <v>330</v>
-      </c>
-      <c r="G87" s="12" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="88" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4365,16 +4368,16 @@
         <v>45698.915277777778</v>
       </c>
       <c r="D88" s="9" t="s">
+        <v>331</v>
+      </c>
+      <c r="E88" s="16" t="s">
         <v>332</v>
       </c>
-      <c r="E88" s="16" t="s">
+      <c r="F88" s="7" t="s">
         <v>333</v>
       </c>
-      <c r="F88" s="7" t="s">
+      <c r="G88" s="7" t="s">
         <v>334</v>
-      </c>
-      <c r="G88" s="7" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="89" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4388,13 +4391,13 @@
         <v>45699.45208333333</v>
       </c>
       <c r="D89" s="14" t="s">
+        <v>335</v>
+      </c>
+      <c r="E89" s="10" t="s">
         <v>336</v>
       </c>
-      <c r="E89" s="10" t="s">
+      <c r="F89" s="12" t="s">
         <v>337</v>
-      </c>
-      <c r="F89" s="12" t="s">
-        <v>338</v>
       </c>
       <c r="G89" s="12"/>
     </row>
@@ -4409,16 +4412,16 @@
         <v>45699.698611111111</v>
       </c>
       <c r="D90" s="9" t="s">
+        <v>338</v>
+      </c>
+      <c r="E90" s="10" t="s">
         <v>339</v>
       </c>
-      <c r="E90" s="10" t="s">
+      <c r="F90" s="7" t="s">
         <v>340</v>
       </c>
-      <c r="F90" s="7" t="s">
+      <c r="G90" s="7" t="s">
         <v>341</v>
-      </c>
-      <c r="G90" s="7" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4432,16 +4435,16 @@
         <v>45699.954861111109</v>
       </c>
       <c r="D91" s="14" t="s">
+        <v>342</v>
+      </c>
+      <c r="E91" s="10" t="s">
         <v>343</v>
       </c>
-      <c r="E91" s="10" t="s">
+      <c r="F91" s="12" t="s">
         <v>344</v>
       </c>
-      <c r="F91" s="12" t="s">
+      <c r="G91" s="12" t="s">
         <v>345</v>
-      </c>
-      <c r="G91" s="12" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="92" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4455,16 +4458,16 @@
         <v>45700.399305555555</v>
       </c>
       <c r="D92" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="E92" s="16" t="s">
         <v>347</v>
       </c>
-      <c r="E92" s="16" t="s">
+      <c r="F92" s="7" t="s">
         <v>348</v>
       </c>
-      <c r="F92" s="7" t="s">
+      <c r="G92" s="7" t="s">
         <v>349</v>
-      </c>
-      <c r="G92" s="7" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4478,16 +4481,16 @@
         <v>45700.749305555553</v>
       </c>
       <c r="D93" s="14" t="s">
+        <v>350</v>
+      </c>
+      <c r="E93" s="16" t="s">
         <v>351</v>
       </c>
-      <c r="E93" s="16" t="s">
+      <c r="F93" s="12" t="s">
         <v>352</v>
       </c>
-      <c r="F93" s="12" t="s">
+      <c r="G93" s="12" t="s">
         <v>353</v>
-      </c>
-      <c r="G93" s="12" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="94" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4501,13 +4504,13 @@
         <v>45700.75</v>
       </c>
       <c r="D94" s="9" t="s">
+        <v>354</v>
+      </c>
+      <c r="E94" s="16" t="s">
         <v>355</v>
       </c>
-      <c r="E94" s="16" t="s">
+      <c r="F94" s="7" t="s">
         <v>356</v>
-      </c>
-      <c r="F94" s="7" t="s">
-        <v>357</v>
       </c>
       <c r="G94" s="7"/>
     </row>
@@ -4522,16 +4525,16 @@
         <v>45700.754166666666</v>
       </c>
       <c r="D95" s="14" t="s">
+        <v>357</v>
+      </c>
+      <c r="E95" s="16" t="s">
         <v>358</v>
       </c>
-      <c r="E95" s="16" t="s">
+      <c r="F95" s="12" t="s">
         <v>359</v>
       </c>
-      <c r="F95" s="12" t="s">
+      <c r="G95" s="12" t="s">
         <v>360</v>
-      </c>
-      <c r="G95" s="12" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="96" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4545,16 +4548,16 @@
         <v>45700.788888888892</v>
       </c>
       <c r="D96" s="9" t="s">
+        <v>361</v>
+      </c>
+      <c r="E96" s="10" t="s">
         <v>362</v>
       </c>
-      <c r="E96" s="10" t="s">
+      <c r="F96" s="7" t="s">
         <v>363</v>
       </c>
-      <c r="F96" s="7" t="s">
+      <c r="G96" s="7" t="s">
         <v>364</v>
-      </c>
-      <c r="G96" s="7" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="97" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4568,13 +4571,13 @@
         <v>45700.792361111111</v>
       </c>
       <c r="D97" s="14" t="s">
+        <v>365</v>
+      </c>
+      <c r="E97" s="16" t="s">
         <v>366</v>
       </c>
-      <c r="E97" s="16" t="s">
+      <c r="F97" s="12" t="s">
         <v>367</v>
-      </c>
-      <c r="F97" s="12" t="s">
-        <v>368</v>
       </c>
       <c r="G97" s="12"/>
     </row>
@@ -4589,16 +4592,16 @@
         <v>45700.793749999997</v>
       </c>
       <c r="D98" s="9" t="s">
+        <v>368</v>
+      </c>
+      <c r="E98" s="16" t="s">
         <v>369</v>
       </c>
-      <c r="E98" s="16" t="s">
+      <c r="F98" s="7" t="s">
         <v>370</v>
       </c>
-      <c r="F98" s="7" t="s">
+      <c r="G98" s="7" t="s">
         <v>371</v>
-      </c>
-      <c r="G98" s="7" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="99" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4612,16 +4615,16 @@
         <v>45700.800000000003</v>
       </c>
       <c r="D99" s="14" t="s">
+        <v>372</v>
+      </c>
+      <c r="E99" s="16" t="s">
         <v>373</v>
       </c>
-      <c r="E99" s="16" t="s">
+      <c r="F99" s="12" t="s">
         <v>374</v>
       </c>
-      <c r="F99" s="12" t="s">
+      <c r="G99" s="12" t="s">
         <v>375</v>
-      </c>
-      <c r="G99" s="12" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="100" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4635,16 +4638,16 @@
         <v>45700.801388888889</v>
       </c>
       <c r="D100" s="9" t="s">
+        <v>376</v>
+      </c>
+      <c r="E100" s="10" t="s">
         <v>377</v>
       </c>
-      <c r="E100" s="10" t="s">
+      <c r="F100" s="7" t="s">
         <v>378</v>
       </c>
-      <c r="F100" s="7" t="s">
+      <c r="G100" s="7" t="s">
         <v>379</v>
-      </c>
-      <c r="G100" s="7" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4658,13 +4661,13 @@
         <v>45700.817361111112</v>
       </c>
       <c r="D101" s="14" t="s">
+        <v>380</v>
+      </c>
+      <c r="E101" s="16" t="s">
         <v>381</v>
       </c>
-      <c r="E101" s="16" t="s">
+      <c r="F101" s="12" t="s">
         <v>382</v>
-      </c>
-      <c r="F101" s="12" t="s">
-        <v>383</v>
       </c>
       <c r="G101" s="12"/>
     </row>
@@ -4679,16 +4682,16 @@
         <v>45700.826388888891</v>
       </c>
       <c r="D102" s="9" t="s">
+        <v>383</v>
+      </c>
+      <c r="E102" s="16" t="s">
         <v>384</v>
       </c>
-      <c r="E102" s="16" t="s">
+      <c r="F102" s="7" t="s">
         <v>385</v>
       </c>
-      <c r="F102" s="7" t="s">
+      <c r="G102" s="7" t="s">
         <v>386</v>
-      </c>
-      <c r="G102" s="7" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="103" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4702,16 +4705,16 @@
         <v>45700.853472222225</v>
       </c>
       <c r="D103" s="14" t="s">
+        <v>387</v>
+      </c>
+      <c r="E103" s="16" t="s">
         <v>388</v>
       </c>
-      <c r="E103" s="16" t="s">
+      <c r="F103" s="12" t="s">
         <v>389</v>
       </c>
-      <c r="F103" s="12" t="s">
+      <c r="G103" s="12" t="s">
         <v>390</v>
-      </c>
-      <c r="G103" s="12" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="104" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4725,16 +4728,16 @@
         <v>45700.866666666669</v>
       </c>
       <c r="D104" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="E104" s="16" t="s">
         <v>392</v>
       </c>
-      <c r="E104" s="16" t="s">
+      <c r="F104" s="7" t="s">
         <v>393</v>
       </c>
-      <c r="F104" s="7" t="s">
+      <c r="G104" s="7" t="s">
         <v>394</v>
-      </c>
-      <c r="G104" s="7" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="105" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4748,16 +4751,16 @@
         <v>45700.873611111114</v>
       </c>
       <c r="D105" s="14" t="s">
+        <v>395</v>
+      </c>
+      <c r="E105" s="10" t="s">
         <v>396</v>
       </c>
-      <c r="E105" s="10" t="s">
+      <c r="F105" s="12" t="s">
         <v>397</v>
       </c>
-      <c r="F105" s="12" t="s">
+      <c r="G105" s="12" t="s">
         <v>398</v>
-      </c>
-      <c r="G105" s="12" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="106" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4771,16 +4774,16 @@
         <v>45700.904861111114</v>
       </c>
       <c r="D106" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="E106" s="16" t="s">
         <v>400</v>
       </c>
-      <c r="E106" s="16" t="s">
+      <c r="F106" s="7" t="s">
         <v>401</v>
       </c>
-      <c r="F106" s="7" t="s">
+      <c r="G106" s="7" t="s">
         <v>402</v>
-      </c>
-      <c r="G106" s="7" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="107" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4794,16 +4797,16 @@
         <v>45701.313888888886</v>
       </c>
       <c r="D107" s="14" t="s">
+        <v>403</v>
+      </c>
+      <c r="E107" s="10" t="s">
         <v>404</v>
       </c>
-      <c r="E107" s="10" t="s">
+      <c r="F107" s="12" t="s">
         <v>405</v>
       </c>
-      <c r="F107" s="12" t="s">
+      <c r="G107" s="12" t="s">
         <v>406</v>
-      </c>
-      <c r="G107" s="12" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="108" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4817,16 +4820,16 @@
         <v>45701.356944444444</v>
       </c>
       <c r="D108" s="9" t="s">
+        <v>407</v>
+      </c>
+      <c r="E108" s="16" t="s">
         <v>408</v>
       </c>
-      <c r="E108" s="16" t="s">
+      <c r="F108" s="7" t="s">
         <v>409</v>
       </c>
-      <c r="F108" s="7" t="s">
+      <c r="G108" s="7" t="s">
         <v>410</v>
-      </c>
-      <c r="G108" s="7" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="109" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4840,13 +4843,13 @@
         <v>45701.39166666667</v>
       </c>
       <c r="D109" s="14" t="s">
+        <v>411</v>
+      </c>
+      <c r="E109" s="10" t="s">
         <v>412</v>
       </c>
-      <c r="E109" s="10" t="s">
+      <c r="F109" s="12" t="s">
         <v>413</v>
-      </c>
-      <c r="F109" s="12" t="s">
-        <v>414</v>
       </c>
       <c r="G109" s="12"/>
     </row>
@@ -4861,16 +4864,16 @@
         <v>45701.416666666664</v>
       </c>
       <c r="D110" s="9" t="s">
+        <v>414</v>
+      </c>
+      <c r="E110" s="10" t="s">
         <v>415</v>
       </c>
-      <c r="E110" s="10" t="s">
+      <c r="F110" s="7" t="s">
         <v>416</v>
       </c>
-      <c r="F110" s="7" t="s">
+      <c r="G110" s="7" t="s">
         <v>417</v>
-      </c>
-      <c r="G110" s="7" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="111" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4884,16 +4887,16 @@
         <v>45701.513888888891</v>
       </c>
       <c r="D111" s="14" t="s">
+        <v>418</v>
+      </c>
+      <c r="E111" s="16" t="s">
         <v>419</v>
       </c>
-      <c r="E111" s="16" t="s">
+      <c r="F111" s="12" t="s">
         <v>420</v>
       </c>
-      <c r="F111" s="12" t="s">
+      <c r="G111" s="12" t="s">
         <v>421</v>
-      </c>
-      <c r="G111" s="12" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="112" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4907,13 +4910,13 @@
         <v>45701.700694444444</v>
       </c>
       <c r="D112" s="9" t="s">
+        <v>422</v>
+      </c>
+      <c r="E112" s="10" t="s">
         <v>423</v>
       </c>
-      <c r="E112" s="10" t="s">
+      <c r="F112" s="7" t="s">
         <v>424</v>
-      </c>
-      <c r="F112" s="7" t="s">
-        <v>425</v>
       </c>
       <c r="G112" s="7"/>
     </row>
@@ -4928,16 +4931,16 @@
         <v>45701.961111111108</v>
       </c>
       <c r="D113" s="14" t="s">
+        <v>425</v>
+      </c>
+      <c r="E113" s="16" t="s">
         <v>426</v>
       </c>
-      <c r="E113" s="16" t="s">
+      <c r="F113" s="12" t="s">
         <v>427</v>
       </c>
-      <c r="F113" s="12" t="s">
+      <c r="G113" s="12" t="s">
         <v>428</v>
-      </c>
-      <c r="G113" s="12" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="114" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4951,16 +4954,16 @@
         <v>45702.586111111108</v>
       </c>
       <c r="D114" s="9" t="s">
+        <v>429</v>
+      </c>
+      <c r="E114" s="16" t="s">
         <v>430</v>
       </c>
-      <c r="E114" s="16" t="s">
+      <c r="F114" s="7" t="s">
         <v>431</v>
       </c>
-      <c r="F114" s="7" t="s">
+      <c r="G114" s="11" t="s">
         <v>432</v>
-      </c>
-      <c r="G114" s="11" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="115" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4974,16 +4977,16 @@
         <v>45702.688194444447</v>
       </c>
       <c r="D115" s="14" t="s">
+        <v>433</v>
+      </c>
+      <c r="E115" s="16" t="s">
         <v>434</v>
       </c>
-      <c r="E115" s="16" t="s">
+      <c r="F115" s="12" t="s">
         <v>435</v>
       </c>
-      <c r="F115" s="12" t="s">
+      <c r="G115" s="12" t="s">
         <v>436</v>
-      </c>
-      <c r="G115" s="12" t="s">
-        <v>437</v>
       </c>
     </row>
     <row r="116" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -4997,16 +5000,16 @@
         <v>45702.945138888892</v>
       </c>
       <c r="D116" s="9" t="s">
+        <v>437</v>
+      </c>
+      <c r="E116" s="16" t="s">
         <v>438</v>
       </c>
-      <c r="E116" s="16" t="s">
+      <c r="F116" s="7" t="s">
         <v>439</v>
       </c>
-      <c r="F116" s="7" t="s">
+      <c r="G116" s="7" t="s">
         <v>440</v>
-      </c>
-      <c r="G116" s="7" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="117" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5020,16 +5023,16 @@
         <v>45703.414583333331</v>
       </c>
       <c r="D117" s="14" t="s">
+        <v>441</v>
+      </c>
+      <c r="E117" s="10" t="s">
         <v>442</v>
       </c>
-      <c r="E117" s="10" t="s">
+      <c r="F117" s="12" t="s">
         <v>443</v>
       </c>
-      <c r="F117" s="12" t="s">
+      <c r="G117" s="12" t="s">
         <v>444</v>
-      </c>
-      <c r="G117" s="12" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="118" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5043,16 +5046,16 @@
         <v>45703.885416666664</v>
       </c>
       <c r="D118" s="9" t="s">
+        <v>445</v>
+      </c>
+      <c r="E118" s="16" t="s">
         <v>446</v>
       </c>
-      <c r="E118" s="16" t="s">
+      <c r="F118" s="7" t="s">
         <v>447</v>
       </c>
-      <c r="F118" s="7" t="s">
+      <c r="G118" s="7" t="s">
         <v>448</v>
-      </c>
-      <c r="G118" s="7" t="s">
-        <v>449</v>
       </c>
     </row>
     <row r="119" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5066,13 +5069,13 @@
         <v>45704.025694444441</v>
       </c>
       <c r="D119" s="14" t="s">
+        <v>449</v>
+      </c>
+      <c r="E119" s="16" t="s">
         <v>450</v>
       </c>
-      <c r="E119" s="16" t="s">
+      <c r="F119" s="12" t="s">
         <v>451</v>
-      </c>
-      <c r="F119" s="12" t="s">
-        <v>452</v>
       </c>
       <c r="G119" s="12"/>
     </row>
@@ -5087,13 +5090,13 @@
         <v>45704.026388888888</v>
       </c>
       <c r="D120" s="9" t="s">
+        <v>452</v>
+      </c>
+      <c r="E120" s="16" t="s">
         <v>453</v>
       </c>
-      <c r="E120" s="16" t="s">
+      <c r="F120" s="7" t="s">
         <v>454</v>
-      </c>
-      <c r="F120" s="7" t="s">
-        <v>455</v>
       </c>
       <c r="G120" s="7"/>
     </row>
@@ -5108,16 +5111,16 @@
         <v>45704.604861111111</v>
       </c>
       <c r="D121" s="14" t="s">
+        <v>455</v>
+      </c>
+      <c r="E121" s="16" t="s">
         <v>456</v>
       </c>
-      <c r="E121" s="16" t="s">
+      <c r="F121" s="12" t="s">
         <v>457</v>
       </c>
-      <c r="F121" s="12" t="s">
+      <c r="G121" s="12" t="s">
         <v>458</v>
-      </c>
-      <c r="G121" s="12" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="122" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5131,16 +5134,16 @@
         <v>45704.694444444445</v>
       </c>
       <c r="D122" s="9" t="s">
+        <v>459</v>
+      </c>
+      <c r="E122" s="16" t="s">
         <v>460</v>
       </c>
-      <c r="E122" s="16" t="s">
+      <c r="F122" s="7" t="s">
         <v>461</v>
       </c>
-      <c r="F122" s="7" t="s">
+      <c r="G122" s="7" t="s">
         <v>462</v>
-      </c>
-      <c r="G122" s="7" t="s">
-        <v>463</v>
       </c>
     </row>
     <row r="123" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5154,16 +5157,16 @@
         <v>45704.870138888888</v>
       </c>
       <c r="D123" s="14" t="s">
+        <v>463</v>
+      </c>
+      <c r="E123" s="10" t="s">
         <v>464</v>
       </c>
-      <c r="E123" s="10" t="s">
+      <c r="F123" s="12" t="s">
         <v>465</v>
       </c>
-      <c r="F123" s="12" t="s">
+      <c r="G123" s="12" t="s">
         <v>466</v>
-      </c>
-      <c r="G123" s="12" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="124" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5177,13 +5180,13 @@
         <v>45704.884722222225</v>
       </c>
       <c r="D124" s="9" t="s">
+        <v>467</v>
+      </c>
+      <c r="E124" s="16" t="s">
         <v>468</v>
       </c>
-      <c r="E124" s="16" t="s">
+      <c r="F124" s="7" t="s">
         <v>469</v>
-      </c>
-      <c r="F124" s="7" t="s">
-        <v>470</v>
       </c>
       <c r="G124" s="7"/>
     </row>
@@ -5198,16 +5201,16 @@
         <v>45704.904166666667</v>
       </c>
       <c r="D125" s="14" t="s">
+        <v>470</v>
+      </c>
+      <c r="E125" s="10" t="s">
         <v>471</v>
       </c>
-      <c r="E125" s="10" t="s">
+      <c r="F125" s="12" t="s">
         <v>472</v>
       </c>
-      <c r="F125" s="12" t="s">
+      <c r="G125" s="12" t="s">
         <v>473</v>
-      </c>
-      <c r="G125" s="12" t="s">
-        <v>474</v>
       </c>
     </row>
     <row r="126" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5221,16 +5224,16 @@
         <v>45705.481249999997</v>
       </c>
       <c r="D126" s="9" t="s">
+        <v>474</v>
+      </c>
+      <c r="E126" s="16" t="s">
         <v>475</v>
       </c>
-      <c r="E126" s="16" t="s">
+      <c r="F126" s="7" t="s">
         <v>476</v>
       </c>
-      <c r="F126" s="7" t="s">
+      <c r="G126" s="7" t="s">
         <v>477</v>
-      </c>
-      <c r="G126" s="7" t="s">
-        <v>478</v>
       </c>
     </row>
     <row r="127" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5244,16 +5247,16 @@
         <v>45705.96875</v>
       </c>
       <c r="D127" s="14" t="s">
+        <v>478</v>
+      </c>
+      <c r="E127" s="16" t="s">
         <v>479</v>
       </c>
-      <c r="E127" s="16" t="s">
+      <c r="F127" s="12" t="s">
         <v>480</v>
       </c>
-      <c r="F127" s="12" t="s">
+      <c r="G127" s="12" t="s">
         <v>481</v>
-      </c>
-      <c r="G127" s="12" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="128" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5267,16 +5270,16 @@
         <v>45706.304861111108</v>
       </c>
       <c r="D128" s="9" t="s">
+        <v>482</v>
+      </c>
+      <c r="E128" s="16" t="s">
         <v>483</v>
       </c>
-      <c r="E128" s="16" t="s">
+      <c r="F128" s="7" t="s">
         <v>484</v>
       </c>
-      <c r="F128" s="7" t="s">
+      <c r="G128" s="7" t="s">
         <v>485</v>
-      </c>
-      <c r="G128" s="7" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="129" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5290,13 +5293,13 @@
         <v>45706.479861111111</v>
       </c>
       <c r="D129" s="14" t="s">
+        <v>486</v>
+      </c>
+      <c r="E129" s="16" t="s">
         <v>487</v>
       </c>
-      <c r="E129" s="16" t="s">
+      <c r="F129" s="12" t="s">
         <v>488</v>
-      </c>
-      <c r="F129" s="12" t="s">
-        <v>489</v>
       </c>
       <c r="G129" s="12"/>
     </row>
@@ -5311,16 +5314,16 @@
         <v>45706.632638888892</v>
       </c>
       <c r="D130" s="9" t="s">
+        <v>489</v>
+      </c>
+      <c r="E130" s="10" t="s">
         <v>490</v>
       </c>
-      <c r="E130" s="10" t="s">
+      <c r="F130" s="7" t="s">
         <v>491</v>
       </c>
-      <c r="F130" s="7" t="s">
+      <c r="G130" s="7" t="s">
         <v>492</v>
-      </c>
-      <c r="G130" s="7" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="131" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5334,16 +5337,16 @@
         <v>45706.658333333333</v>
       </c>
       <c r="D131" s="14" t="s">
+        <v>493</v>
+      </c>
+      <c r="E131" s="16" t="s">
         <v>494</v>
       </c>
-      <c r="E131" s="16" t="s">
+      <c r="F131" s="12" t="s">
         <v>495</v>
       </c>
-      <c r="F131" s="12" t="s">
+      <c r="G131" s="12" t="s">
         <v>496</v>
-      </c>
-      <c r="G131" s="12" t="s">
-        <v>497</v>
       </c>
     </row>
     <row r="132" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5357,16 +5360,16 @@
         <v>45706.714583333334</v>
       </c>
       <c r="D132" s="9" t="s">
+        <v>497</v>
+      </c>
+      <c r="E132" s="16" t="s">
         <v>498</v>
       </c>
-      <c r="E132" s="16" t="s">
+      <c r="F132" s="7" t="s">
         <v>499</v>
       </c>
-      <c r="F132" s="7" t="s">
+      <c r="G132" s="7" t="s">
         <v>500</v>
-      </c>
-      <c r="G132" s="7" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="133" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5380,13 +5383,13 @@
         <v>45707.393750000003</v>
       </c>
       <c r="D133" s="14" t="s">
+        <v>501</v>
+      </c>
+      <c r="E133" s="16" t="s">
         <v>502</v>
       </c>
-      <c r="E133" s="16" t="s">
+      <c r="F133" s="12" t="s">
         <v>503</v>
-      </c>
-      <c r="F133" s="12" t="s">
-        <v>504</v>
       </c>
       <c r="G133" s="12"/>
     </row>
@@ -5401,16 +5404,16 @@
         <v>45707.679861111108</v>
       </c>
       <c r="D134" s="9" t="s">
+        <v>504</v>
+      </c>
+      <c r="E134" s="10" t="s">
         <v>505</v>
       </c>
-      <c r="E134" s="10" t="s">
+      <c r="F134" s="7" t="s">
         <v>506</v>
       </c>
-      <c r="F134" s="7" t="s">
+      <c r="G134" s="7" t="s">
         <v>507</v>
-      </c>
-      <c r="G134" s="7" t="s">
-        <v>508</v>
       </c>
     </row>
     <row r="135" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5424,16 +5427,16 @@
         <v>45707.68472222222</v>
       </c>
       <c r="D135" s="14" t="s">
+        <v>508</v>
+      </c>
+      <c r="E135" s="10" t="s">
         <v>509</v>
       </c>
-      <c r="E135" s="10" t="s">
+      <c r="F135" s="12" t="s">
         <v>510</v>
       </c>
-      <c r="F135" s="12" t="s">
+      <c r="G135" s="12" t="s">
         <v>511</v>
-      </c>
-      <c r="G135" s="12" t="s">
-        <v>512</v>
       </c>
     </row>
     <row r="136" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5447,13 +5450,13 @@
         <v>45707.76666666667</v>
       </c>
       <c r="D136" s="9" t="s">
+        <v>512</v>
+      </c>
+      <c r="E136" s="16" t="s">
         <v>513</v>
       </c>
-      <c r="E136" s="16" t="s">
+      <c r="F136" s="7" t="s">
         <v>514</v>
-      </c>
-      <c r="F136" s="7" t="s">
-        <v>515</v>
       </c>
       <c r="G136" s="7"/>
     </row>
@@ -5468,13 +5471,13 @@
         <v>45707.875</v>
       </c>
       <c r="D137" s="14" t="s">
+        <v>515</v>
+      </c>
+      <c r="E137" s="10" t="s">
         <v>516</v>
       </c>
-      <c r="E137" s="10" t="s">
+      <c r="F137" s="12" t="s">
         <v>517</v>
-      </c>
-      <c r="F137" s="12" t="s">
-        <v>518</v>
       </c>
       <c r="G137" s="12"/>
     </row>
@@ -5489,13 +5492,13 @@
         <v>45707.888888888891</v>
       </c>
       <c r="D138" s="9" t="s">
+        <v>518</v>
+      </c>
+      <c r="E138" s="16" t="s">
         <v>519</v>
       </c>
-      <c r="E138" s="16" t="s">
+      <c r="F138" s="7" t="s">
         <v>520</v>
-      </c>
-      <c r="F138" s="7" t="s">
-        <v>521</v>
       </c>
       <c r="G138" s="7"/>
     </row>
@@ -5510,13 +5513,13 @@
         <v>45708.465277777781</v>
       </c>
       <c r="D139" s="14" t="s">
+        <v>521</v>
+      </c>
+      <c r="E139" s="16" t="s">
         <v>522</v>
       </c>
-      <c r="E139" s="16" t="s">
+      <c r="F139" s="12" t="s">
         <v>523</v>
-      </c>
-      <c r="F139" s="12" t="s">
-        <v>524</v>
       </c>
       <c r="G139" s="12"/>
     </row>
@@ -5531,16 +5534,16 @@
         <v>45708.57708333333</v>
       </c>
       <c r="D140" s="9" t="s">
+        <v>524</v>
+      </c>
+      <c r="E140" s="16" t="s">
         <v>525</v>
       </c>
-      <c r="E140" s="16" t="s">
+      <c r="F140" s="7" t="s">
         <v>526</v>
       </c>
-      <c r="F140" s="7" t="s">
+      <c r="G140" s="7" t="s">
         <v>527</v>
-      </c>
-      <c r="G140" s="7" t="s">
-        <v>528</v>
       </c>
     </row>
     <row r="141" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5554,13 +5557,13 @@
         <v>45708.613888888889</v>
       </c>
       <c r="D141" s="14" t="s">
+        <v>528</v>
+      </c>
+      <c r="E141" s="16" t="s">
         <v>529</v>
       </c>
-      <c r="E141" s="16" t="s">
+      <c r="F141" s="12" t="s">
         <v>530</v>
-      </c>
-      <c r="F141" s="12" t="s">
-        <v>531</v>
       </c>
       <c r="G141" s="12"/>
     </row>
@@ -5575,16 +5578,16 @@
         <v>45708.713888888888</v>
       </c>
       <c r="D142" s="9" t="s">
+        <v>531</v>
+      </c>
+      <c r="E142" s="16" t="s">
         <v>532</v>
       </c>
-      <c r="E142" s="16" t="s">
+      <c r="F142" s="7" t="s">
         <v>533</v>
       </c>
-      <c r="F142" s="7" t="s">
+      <c r="G142" s="7" t="s">
         <v>534</v>
-      </c>
-      <c r="G142" s="7" t="s">
-        <v>535</v>
       </c>
     </row>
     <row r="143" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5598,16 +5601,16 @@
         <v>45708.728472222225</v>
       </c>
       <c r="D143" s="14" t="s">
+        <v>535</v>
+      </c>
+      <c r="E143" s="16" t="s">
         <v>536</v>
       </c>
-      <c r="E143" s="16" t="s">
+      <c r="F143" s="12" t="s">
         <v>537</v>
       </c>
-      <c r="F143" s="12" t="s">
+      <c r="G143" s="12" t="s">
         <v>538</v>
-      </c>
-      <c r="G143" s="12" t="s">
-        <v>539</v>
       </c>
     </row>
     <row r="144" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5621,16 +5624,16 @@
         <v>45708.731944444444</v>
       </c>
       <c r="D144" s="9" t="s">
+        <v>539</v>
+      </c>
+      <c r="E144" s="16" t="s">
         <v>540</v>
       </c>
-      <c r="E144" s="16" t="s">
+      <c r="F144" s="7" t="s">
         <v>541</v>
       </c>
-      <c r="F144" s="7" t="s">
+      <c r="G144" s="7" t="s">
         <v>542</v>
-      </c>
-      <c r="G144" s="7" t="s">
-        <v>543</v>
       </c>
     </row>
     <row r="145" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5644,16 +5647,16 @@
         <v>45708.742361111108</v>
       </c>
       <c r="D145" s="14" t="s">
+        <v>543</v>
+      </c>
+      <c r="E145" s="10" t="s">
         <v>544</v>
       </c>
-      <c r="E145" s="10" t="s">
+      <c r="F145" s="12" t="s">
         <v>545</v>
       </c>
-      <c r="F145" s="12" t="s">
+      <c r="G145" s="12" t="s">
         <v>546</v>
-      </c>
-      <c r="G145" s="12" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="146" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5667,16 +5670,16 @@
         <v>45708.753472222219</v>
       </c>
       <c r="D146" s="9" t="s">
+        <v>547</v>
+      </c>
+      <c r="E146" s="16" t="s">
         <v>548</v>
       </c>
-      <c r="E146" s="16" t="s">
+      <c r="F146" s="7" t="s">
         <v>549</v>
       </c>
-      <c r="F146" s="7" t="s">
+      <c r="G146" s="7" t="s">
         <v>550</v>
-      </c>
-      <c r="G146" s="7" t="s">
-        <v>551</v>
       </c>
     </row>
     <row r="147" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5690,13 +5693,13 @@
         <v>45708.822916666664</v>
       </c>
       <c r="D147" s="14" t="s">
+        <v>551</v>
+      </c>
+      <c r="E147" s="16" t="s">
         <v>552</v>
       </c>
-      <c r="E147" s="16" t="s">
+      <c r="F147" s="12" t="s">
         <v>553</v>
-      </c>
-      <c r="F147" s="12" t="s">
-        <v>554</v>
       </c>
       <c r="G147" s="12"/>
     </row>
@@ -5711,13 +5714,13 @@
         <v>45708.874305555553</v>
       </c>
       <c r="D148" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="E148" s="16" t="s">
         <v>555</v>
       </c>
-      <c r="E148" s="16" t="s">
+      <c r="F148" s="7" t="s">
         <v>556</v>
-      </c>
-      <c r="F148" s="7" t="s">
-        <v>557</v>
       </c>
       <c r="G148" s="7"/>
     </row>
@@ -5732,13 +5735,13 @@
         <v>45709.375</v>
       </c>
       <c r="D149" s="14" t="s">
+        <v>557</v>
+      </c>
+      <c r="E149" s="16" t="s">
         <v>558</v>
       </c>
-      <c r="E149" s="16" t="s">
+      <c r="F149" s="12" t="s">
         <v>559</v>
-      </c>
-      <c r="F149" s="12" t="s">
-        <v>560</v>
       </c>
       <c r="G149" s="12"/>
     </row>
@@ -5753,16 +5756,16 @@
         <v>45709.443749999999</v>
       </c>
       <c r="D150" s="9" t="s">
+        <v>560</v>
+      </c>
+      <c r="E150" s="16" t="s">
         <v>561</v>
       </c>
-      <c r="E150" s="16" t="s">
+      <c r="F150" s="7" t="s">
         <v>562</v>
       </c>
-      <c r="F150" s="7" t="s">
+      <c r="G150" s="7" t="s">
         <v>563</v>
-      </c>
-      <c r="G150" s="7" t="s">
-        <v>564</v>
       </c>
     </row>
     <row r="151" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5776,16 +5779,16 @@
         <v>45709.461805555555</v>
       </c>
       <c r="D151" s="14" t="s">
+        <v>564</v>
+      </c>
+      <c r="E151" s="16" t="s">
         <v>565</v>
       </c>
-      <c r="E151" s="16" t="s">
+      <c r="F151" s="12" t="s">
         <v>566</v>
       </c>
-      <c r="F151" s="12" t="s">
+      <c r="G151" s="12" t="s">
         <v>567</v>
-      </c>
-      <c r="G151" s="12" t="s">
-        <v>568</v>
       </c>
     </row>
     <row r="152" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5799,16 +5802,16 @@
         <v>45709.756944444445</v>
       </c>
       <c r="D152" s="9" t="s">
+        <v>568</v>
+      </c>
+      <c r="E152" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="E152" s="16" t="s">
+      <c r="F152" s="7" t="s">
         <v>570</v>
       </c>
-      <c r="F152" s="7" t="s">
+      <c r="G152" s="7" t="s">
         <v>571</v>
-      </c>
-      <c r="G152" s="7" t="s">
-        <v>572</v>
       </c>
     </row>
     <row r="153" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5822,16 +5825,16 @@
         <v>45709.758333333331</v>
       </c>
       <c r="D153" s="14" t="s">
+        <v>572</v>
+      </c>
+      <c r="E153" s="16" t="s">
         <v>573</v>
       </c>
-      <c r="E153" s="16" t="s">
+      <c r="F153" s="12" t="s">
         <v>574</v>
       </c>
-      <c r="F153" s="12" t="s">
+      <c r="G153" s="12" t="s">
         <v>575</v>
-      </c>
-      <c r="G153" s="12" t="s">
-        <v>576</v>
       </c>
     </row>
     <row r="154" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5845,13 +5848,13 @@
         <v>45709.803472222222</v>
       </c>
       <c r="D154" s="9" t="s">
+        <v>576</v>
+      </c>
+      <c r="E154" s="16" t="s">
         <v>577</v>
       </c>
-      <c r="E154" s="16" t="s">
+      <c r="F154" s="7" t="s">
         <v>578</v>
-      </c>
-      <c r="F154" s="7" t="s">
-        <v>579</v>
       </c>
       <c r="G154" s="7"/>
     </row>
@@ -5866,16 +5869,16 @@
         <v>45709.904861111114</v>
       </c>
       <c r="D155" s="14" t="s">
+        <v>579</v>
+      </c>
+      <c r="E155" s="16" t="s">
         <v>580</v>
       </c>
-      <c r="E155" s="16" t="s">
+      <c r="F155" s="12" t="s">
         <v>581</v>
       </c>
-      <c r="F155" s="12" t="s">
+      <c r="G155" s="12" t="s">
         <v>582</v>
-      </c>
-      <c r="G155" s="12" t="s">
-        <v>583</v>
       </c>
     </row>
     <row r="156" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5889,13 +5892,13 @@
         <v>45709.956250000003</v>
       </c>
       <c r="D156" s="9" t="s">
+        <v>583</v>
+      </c>
+      <c r="E156" s="16" t="s">
         <v>584</v>
       </c>
-      <c r="E156" s="16" t="s">
+      <c r="F156" s="7" t="s">
         <v>585</v>
-      </c>
-      <c r="F156" s="7" t="s">
-        <v>586</v>
       </c>
       <c r="G156" s="7"/>
     </row>
@@ -5910,16 +5913,16 @@
         <v>45710.475694444445</v>
       </c>
       <c r="D157" s="14" t="s">
+        <v>586</v>
+      </c>
+      <c r="E157" s="16" t="s">
         <v>587</v>
       </c>
-      <c r="E157" s="16" t="s">
+      <c r="F157" s="12" t="s">
         <v>588</v>
       </c>
-      <c r="F157" s="12" t="s">
+      <c r="G157" s="12" t="s">
         <v>589</v>
-      </c>
-      <c r="G157" s="12" t="s">
-        <v>590</v>
       </c>
     </row>
     <row r="158" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5933,16 +5936,16 @@
         <v>45710.479861111111</v>
       </c>
       <c r="D158" s="9" t="s">
+        <v>590</v>
+      </c>
+      <c r="E158" s="16" t="s">
         <v>591</v>
       </c>
-      <c r="E158" s="16" t="s">
+      <c r="F158" s="7" t="s">
         <v>592</v>
       </c>
-      <c r="F158" s="7" t="s">
+      <c r="G158" s="7" t="s">
         <v>593</v>
-      </c>
-      <c r="G158" s="7" t="s">
-        <v>594</v>
       </c>
     </row>
     <row r="159" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5956,16 +5959,16 @@
         <v>45710.686805555553</v>
       </c>
       <c r="D159" s="14" t="s">
+        <v>594</v>
+      </c>
+      <c r="E159" s="16" t="s">
         <v>595</v>
       </c>
-      <c r="E159" s="16" t="s">
+      <c r="F159" s="12" t="s">
         <v>596</v>
       </c>
-      <c r="F159" s="12" t="s">
+      <c r="G159" s="12" t="s">
         <v>597</v>
-      </c>
-      <c r="G159" s="12" t="s">
-        <v>598</v>
       </c>
     </row>
     <row r="160" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5979,16 +5982,16 @@
         <v>45710.75</v>
       </c>
       <c r="D160" s="9" t="s">
+        <v>598</v>
+      </c>
+      <c r="E160" s="16" t="s">
         <v>599</v>
       </c>
-      <c r="E160" s="16" t="s">
+      <c r="F160" s="7" t="s">
         <v>600</v>
       </c>
-      <c r="F160" s="7" t="s">
+      <c r="G160" s="7" t="s">
         <v>601</v>
-      </c>
-      <c r="G160" s="7" t="s">
-        <v>602</v>
       </c>
     </row>
     <row r="161" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -6002,16 +6005,16 @@
         <v>45710.774305555555</v>
       </c>
       <c r="D161" s="14" t="s">
+        <v>602</v>
+      </c>
+      <c r="E161" s="16" t="s">
         <v>603</v>
       </c>
-      <c r="E161" s="16" t="s">
+      <c r="F161" s="12" t="s">
         <v>604</v>
       </c>
-      <c r="F161" s="12" t="s">
+      <c r="G161" s="12" t="s">
         <v>605</v>
-      </c>
-      <c r="G161" s="12" t="s">
-        <v>606</v>
       </c>
     </row>
     <row r="162" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -6025,13 +6028,13 @@
         <v>45710.988194444442</v>
       </c>
       <c r="D162" s="9" t="s">
+        <v>606</v>
+      </c>
+      <c r="E162" s="16" t="s">
         <v>607</v>
       </c>
-      <c r="E162" s="16" t="s">
+      <c r="F162" s="7" t="s">
         <v>608</v>
-      </c>
-      <c r="F162" s="7" t="s">
-        <v>609</v>
       </c>
       <c r="G162" s="7"/>
     </row>
@@ -6046,16 +6049,16 @@
         <v>45710.995833333334</v>
       </c>
       <c r="D163" s="14" t="s">
+        <v>609</v>
+      </c>
+      <c r="E163" s="16" t="s">
         <v>610</v>
       </c>
-      <c r="E163" s="16" t="s">
+      <c r="F163" s="12" t="s">
         <v>611</v>
       </c>
-      <c r="F163" s="12" t="s">
+      <c r="G163" s="12" t="s">
         <v>612</v>
-      </c>
-      <c r="G163" s="12" t="s">
-        <v>613</v>
       </c>
     </row>
     <row r="164" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -6069,13 +6072,13 @@
         <v>45711.038888888892</v>
       </c>
       <c r="D164" s="9" t="s">
+        <v>613</v>
+      </c>
+      <c r="E164" s="16" t="s">
         <v>614</v>
       </c>
-      <c r="E164" s="16" t="s">
+      <c r="F164" s="7" t="s">
         <v>615</v>
-      </c>
-      <c r="F164" s="7" t="s">
-        <v>616</v>
       </c>
       <c r="G164" s="7"/>
     </row>
@@ -6090,16 +6093,16 @@
         <v>45711.074999999997</v>
       </c>
       <c r="D165" s="14" t="s">
+        <v>616</v>
+      </c>
+      <c r="E165" s="16" t="s">
         <v>617</v>
       </c>
-      <c r="E165" s="16" t="s">
+      <c r="F165" s="12" t="s">
         <v>618</v>
       </c>
-      <c r="F165" s="12" t="s">
+      <c r="G165" s="12" t="s">
         <v>619</v>
-      </c>
-      <c r="G165" s="12" t="s">
-        <v>620</v>
       </c>
     </row>
     <row r="166" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -6113,16 +6116,16 @@
         <v>45711.506944444445</v>
       </c>
       <c r="D166" s="9" t="s">
+        <v>620</v>
+      </c>
+      <c r="E166" s="16" t="s">
         <v>621</v>
       </c>
-      <c r="E166" s="16" t="s">
+      <c r="F166" s="7" t="s">
         <v>622</v>
       </c>
-      <c r="F166" s="7" t="s">
+      <c r="G166" s="11" t="s">
         <v>623</v>
-      </c>
-      <c r="G166" s="11" t="s">
-        <v>624</v>
       </c>
     </row>
     <row r="167" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -6136,13 +6139,13 @@
         <v>45711.522222222222</v>
       </c>
       <c r="D167" s="14" t="s">
+        <v>624</v>
+      </c>
+      <c r="E167" s="16" t="s">
         <v>625</v>
       </c>
-      <c r="E167" s="16" t="s">
+      <c r="F167" s="12" t="s">
         <v>626</v>
-      </c>
-      <c r="F167" s="12" t="s">
-        <v>627</v>
       </c>
       <c r="G167" s="12"/>
     </row>
@@ -6157,16 +6160,16 @@
         <v>45711.522222222222</v>
       </c>
       <c r="D168" s="11" t="s">
+        <v>627</v>
+      </c>
+      <c r="E168" s="16" t="s">
         <v>628</v>
       </c>
-      <c r="E168" s="16" t="s">
+      <c r="F168" s="7" t="s">
         <v>629</v>
       </c>
-      <c r="F168" s="7" t="s">
+      <c r="G168" s="11" t="s">
         <v>630</v>
-      </c>
-      <c r="G168" s="11" t="s">
-        <v>631</v>
       </c>
     </row>
     <row r="169" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -6180,13 +6183,13 @@
         <v>45711.522222222222</v>
       </c>
       <c r="D169" s="11" t="s">
+        <v>631</v>
+      </c>
+      <c r="E169" s="16" t="s">
         <v>632</v>
       </c>
-      <c r="E169" s="16" t="s">
+      <c r="F169" s="7" t="s">
         <v>633</v>
-      </c>
-      <c r="F169" s="7" t="s">
-        <v>634</v>
       </c>
       <c r="G169" s="7"/>
     </row>
@@ -6201,13 +6204,13 @@
         <v>45711.643055555556</v>
       </c>
       <c r="D170" s="11" t="s">
+        <v>634</v>
+      </c>
+      <c r="E170" s="16" t="s">
         <v>635</v>
       </c>
-      <c r="E170" s="16" t="s">
+      <c r="F170" s="7" t="s">
         <v>636</v>
-      </c>
-      <c r="F170" s="7" t="s">
-        <v>637</v>
       </c>
       <c r="G170" s="7"/>
     </row>
@@ -6223,10 +6226,12 @@
     <hyperlink ref="G168" r:id="rId8" display="https://sd36-my.sharepoint.com/personal/yash_jain_surreyschools_ca/Documents/Apps/Microsoft Forms/Grad Tag/Question/Adiv_IMG_GT.jpg" xr:uid="{02CE30A4-A72F-405C-9A20-61FE58BCA6A0}"/>
     <hyperlink ref="D169" r:id="rId9" display="mailto:rs01.edwards@surreyschools.ca" xr:uid="{AE16740D-0E6F-4C05-9B92-93B297C2EC32}"/>
     <hyperlink ref="D170" r:id="rId10" display="mailto:mb01.sanchez@surreyschools.ca" xr:uid="{FB0452C6-BDCF-4063-92DD-348D3AF7B832}"/>
+    <hyperlink ref="G86" r:id="rId11" xr:uid="{2055DE76-4A48-42A3-B831-2CED858F4029}"/>
+    <hyperlink ref="F86" r:id="rId12" xr:uid="{7FF69593-D1D9-42CB-9EB0-E137FDE73E1A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId11"/>
+    <tablePart r:id="rId13"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>